<commit_message>
Final version of thresholds paper
</commit_message>
<xml_diff>
--- a/AnalysisData/Literature/FarrellEtAl2012.xlsx
+++ b/AnalysisData/Literature/FarrellEtAl2012.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="103">
   <si>
     <t>Run</t>
   </si>
@@ -335,6 +335,9 @@
   </si>
   <si>
     <t>NaN</t>
+  </si>
+  <si>
+    <t>Dsigmatrap_mm</t>
   </si>
 </sst>
 </file>
@@ -1474,11 +1477,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1014240016"/>
-        <c:axId val="1013413184"/>
+        <c:axId val="-263029472"/>
+        <c:axId val="-234668368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1014240016"/>
+        <c:axId val="-263029472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,6 +1561,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1594,12 +1598,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1013413184"/>
+        <c:crossAx val="-234668368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1013413184"/>
+        <c:axId val="-234668368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1716,7 +1720,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1014240016"/>
+        <c:crossAx val="-263029472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2678,10 +2682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2691,9 +2695,10 @@
     <col min="5" max="5" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>93</v>
       </c>
@@ -2718,8 +2723,11 @@
       <c r="H1" s="11" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2744,8 +2752,11 @@
       <c r="H2">
         <v>0.33400000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>1.554</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2770,8 +2781,11 @@
       <c r="H3">
         <v>0.27100000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>1.526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2796,8 +2810,11 @@
       <c r="H4">
         <v>0.26400000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2822,8 +2839,11 @@
       <c r="H5">
         <v>0.26100000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>1.4570000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2848,8 +2868,11 @@
       <c r="H6">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2874,8 +2897,11 @@
       <c r="H7">
         <v>0.28499999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>1.4350000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2900,8 +2926,11 @@
       <c r="H8">
         <v>0.26600000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>1.571</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2926,8 +2955,11 @@
       <c r="H9">
         <v>0.22500000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>1.4259999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2952,8 +2984,11 @@
       <c r="H10">
         <v>0.22800000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2978,8 +3013,11 @@
       <c r="H11">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>1.425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -3004,8 +3042,11 @@
       <c r="H12">
         <v>0.24399999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <v>1.4019999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3030,8 +3071,11 @@
       <c r="H13">
         <v>0.251</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <v>1.4179999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -3056,8 +3100,11 @@
       <c r="H14">
         <v>0.27300000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <v>1.554</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -3082,8 +3129,11 @@
       <c r="H15">
         <v>0.24099999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>1.4319999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3108,8 +3158,11 @@
       <c r="H16">
         <v>0.251</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>1.4219999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -3134,8 +3187,11 @@
       <c r="H17">
         <v>0.248</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <v>1.417</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -3160,8 +3216,11 @@
       <c r="H18">
         <v>0.252</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4</v>
       </c>
@@ -3186,8 +3245,11 @@
       <c r="H19">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <v>1.4410000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4</v>
       </c>
@@ -3212,8 +3274,11 @@
       <c r="H20">
         <v>0.29599999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <v>1.4019999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4</v>
       </c>
@@ -3238,8 +3303,11 @@
       <c r="H21">
         <v>0.29199999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21">
+        <v>1.3740000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -3264,8 +3332,11 @@
       <c r="H22">
         <v>0.29599999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22">
+        <v>1.347</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>4</v>
       </c>
@@ -3290,8 +3361,11 @@
       <c r="H23">
         <v>0.29499999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23">
+        <v>1.3819999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>4</v>
       </c>
@@ -3316,8 +3390,11 @@
       <c r="H24">
         <v>0.307</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <v>1.349</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>5</v>
       </c>
@@ -3342,8 +3419,11 @@
       <c r="H25">
         <v>0.32500000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <v>1.4319999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>5</v>
       </c>
@@ -3368,8 +3448,11 @@
       <c r="H26">
         <v>0.28799999999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26">
+        <v>1.385</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>5</v>
       </c>
@@ -3394,8 +3477,11 @@
       <c r="H27">
         <v>0.27600000000000002</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>5</v>
       </c>
@@ -3420,8 +3506,11 @@
       <c r="H28">
         <v>0.29199999999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28">
+        <v>1.341</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>5</v>
       </c>
@@ -3446,8 +3535,11 @@
       <c r="H29">
         <v>0.29199999999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29">
+        <v>1.335</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>5</v>
       </c>
@@ -3472,8 +3564,11 @@
       <c r="H30">
         <v>0.28499999999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30">
+        <v>1.4570000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>6</v>
       </c>
@@ -3498,8 +3593,11 @@
       <c r="H31">
         <v>0.308</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31">
+        <v>1.4690000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>6</v>
       </c>
@@ -3524,8 +3622,11 @@
       <c r="H32">
         <v>0.26900000000000002</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32">
+        <v>1.409</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>6</v>
       </c>
@@ -3550,8 +3651,11 @@
       <c r="H33">
         <v>0.26700000000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33">
+        <v>1.373</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>6</v>
       </c>
@@ -3576,8 +3680,11 @@
       <c r="H34">
         <v>0.27500000000000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34">
+        <v>1.339</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>6</v>
       </c>
@@ -3602,8 +3709,11 @@
       <c r="H35">
         <v>0.28899999999999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35">
+        <v>1.325</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>6</v>
       </c>
@@ -3628,8 +3738,11 @@
       <c r="H36">
         <v>0.29699999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36">
+        <v>1.3169999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>7</v>
       </c>
@@ -3654,8 +3767,11 @@
       <c r="H37">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37">
+        <v>1.484</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>7</v>
       </c>
@@ -3680,8 +3796,11 @@
       <c r="H38">
         <v>0.27300000000000002</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38">
+        <v>1.417</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>7</v>
       </c>
@@ -3706,8 +3825,11 @@
       <c r="H39">
         <v>0.29099999999999998</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39">
+        <v>1.401</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>7</v>
       </c>
@@ -3732,8 +3854,11 @@
       <c r="H40">
         <v>0.28599999999999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40">
+        <v>1.3560000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>7</v>
       </c>
@@ -3758,8 +3883,11 @@
       <c r="H41">
         <v>0.30299999999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41">
+        <v>1.349</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>7</v>
       </c>
@@ -3784,8 +3912,11 @@
       <c r="H42" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>8</v>
       </c>
@@ -3810,8 +3941,11 @@
       <c r="H43">
         <v>0.33700000000000002</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43">
+        <v>1.466</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>8</v>
       </c>
@@ -3836,8 +3970,11 @@
       <c r="H44">
         <v>0.28699999999999998</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44">
+        <v>1.427</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>8</v>
       </c>
@@ -3862,8 +3999,11 @@
       <c r="H45">
         <v>0.27900000000000003</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45">
+        <v>1.365</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>8</v>
       </c>
@@ -3888,8 +4028,11 @@
       <c r="H46">
         <v>0.29199999999999998</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46">
+        <v>1.351</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>8</v>
       </c>
@@ -3914,8 +4057,11 @@
       <c r="H47">
         <v>0.29099999999999998</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47">
+        <v>1.3540000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>8</v>
       </c>
@@ -3940,8 +4086,11 @@
       <c r="H48">
         <v>0.248</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48">
+        <v>1.496</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>9</v>
       </c>
@@ -3966,8 +4115,11 @@
       <c r="H49">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>9</v>
       </c>
@@ -3992,8 +4144,11 @@
       <c r="H50">
         <v>0.29399999999999998</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50">
+        <v>1.4419999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>9</v>
       </c>
@@ -4018,8 +4173,11 @@
       <c r="H51">
         <v>0.27800000000000002</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51">
+        <v>1.383</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>9</v>
       </c>
@@ -4044,8 +4202,11 @@
       <c r="H52">
         <v>0.29099999999999998</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52">
+        <v>1.3620000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>9</v>
       </c>
@@ -4070,8 +4231,11 @@
       <c r="H53">
         <v>0.30199999999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53">
+        <v>1.355</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>9</v>
       </c>
@@ -4096,8 +4260,11 @@
       <c r="H54">
         <v>0.30099999999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54">
+        <v>1.331</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>10</v>
       </c>
@@ -4122,8 +4289,11 @@
       <c r="H55">
         <v>0.35599999999999998</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55">
+        <v>1.5980000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>10</v>
       </c>
@@ -4148,8 +4318,11 @@
       <c r="H56">
         <v>0.28699999999999998</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56">
+        <v>1.5229999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>10</v>
       </c>
@@ -4174,8 +4347,11 @@
       <c r="H57">
         <v>0.28699999999999998</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57">
+        <v>1.4670000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>10</v>
       </c>
@@ -4200,8 +4376,11 @@
       <c r="H58">
         <v>0.29599999999999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58">
+        <v>1.427</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>10</v>
       </c>
@@ -4226,8 +4405,11 @@
       <c r="H59">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59">
+        <v>1.391</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>10</v>
       </c>
@@ -4252,8 +4434,11 @@
       <c r="H60">
         <v>0.32300000000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60">
+        <v>1.355</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>11</v>
       </c>
@@ -4278,8 +4463,11 @@
       <c r="H61">
         <v>0.28899999999999998</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I61">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>11</v>
       </c>
@@ -4304,8 +4492,11 @@
       <c r="H62">
         <v>0.248</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62">
+        <v>1.468</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>11</v>
       </c>
@@ -4330,8 +4521,11 @@
       <c r="H63">
         <v>0.249</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63">
+        <v>1.427</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>11</v>
       </c>
@@ -4356,8 +4550,11 @@
       <c r="H64">
         <v>0.25700000000000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64">
+        <v>1.373</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>11</v>
       </c>
@@ -4382,8 +4579,11 @@
       <c r="H65">
         <v>0.27300000000000002</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65">
+        <v>1.3520000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>11</v>
       </c>
@@ -4408,8 +4608,11 @@
       <c r="H66">
         <v>0.29199999999999998</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66">
+        <v>1.3480000000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>12</v>
       </c>
@@ -4434,8 +4637,11 @@
       <c r="H67">
         <v>0.42899999999999999</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67">
+        <v>1.605</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>12</v>
       </c>
@@ -4460,8 +4666,11 @@
       <c r="H68">
         <v>0.36099999999999999</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68">
+        <v>1.6060000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>12</v>
       </c>
@@ -4486,8 +4695,11 @@
       <c r="H69">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>12</v>
       </c>
@@ -4512,8 +4724,11 @@
       <c r="H70">
         <v>0.376</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70">
+        <v>1.4950000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>12</v>
       </c>
@@ -4538,8 +4753,11 @@
       <c r="H71">
         <v>0.373</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71">
+        <v>1.4419999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>12</v>
       </c>
@@ -4564,8 +4782,11 @@
       <c r="H72">
         <v>0.39500000000000002</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72">
+        <v>1.413</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>13</v>
       </c>
@@ -4590,8 +4811,11 @@
       <c r="H73">
         <v>0.44500000000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73">
+        <v>1.579</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>13</v>
       </c>
@@ -4616,8 +4840,11 @@
       <c r="H74">
         <v>0.35799999999999998</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74">
+        <v>1.6220000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>13</v>
       </c>
@@ -4642,8 +4869,11 @@
       <c r="H75">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75">
+        <v>1.512</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>13</v>
       </c>
@@ -4668,8 +4898,11 @@
       <c r="H76">
         <v>0.372</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76">
+        <v>1.492</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>13</v>
       </c>
@@ -4694,8 +4927,11 @@
       <c r="H77">
         <v>0.36799999999999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77">
+        <v>1.4670000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>13</v>
       </c>
@@ -4720,8 +4956,11 @@
       <c r="H78">
         <v>0.38600000000000001</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I78">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>14</v>
       </c>
@@ -4746,8 +4985,11 @@
       <c r="H79">
         <v>0.439</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I79">
+        <v>1.6419999999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>14</v>
       </c>
@@ -4772,8 +5014,11 @@
       <c r="H80">
         <v>0.35799999999999998</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I80">
+        <v>1.627</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>14</v>
       </c>
@@ -4798,8 +5043,11 @@
       <c r="H81">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I81">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>14</v>
       </c>
@@ -4824,8 +5072,11 @@
       <c r="H82">
         <v>0.36199999999999999</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I82">
+        <v>1.5049999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>14</v>
       </c>
@@ -4850,8 +5101,11 @@
       <c r="H83">
         <v>0.36099999999999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I83">
+        <v>1.462</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>14</v>
       </c>
@@ -4875,6 +5129,9 @@
       </c>
       <c r="H84">
         <v>0.39600000000000002</v>
+      </c>
+      <c r="I84">
+        <v>1.379</v>
       </c>
     </row>
   </sheetData>
@@ -4887,8 +5144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P276"/>
   <sheetViews>
-    <sheetView topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="E234" sqref="E234:J234"/>
+    <sheetView topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="E235" sqref="E235:J235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>